<commit_message>
reorganize the grid frequency
去除低於59.5Hz的頻率
</commit_message>
<xml_diff>
--- a/grid_frequency_EdReg_nonemergency.xlsx
+++ b/grid_frequency_EdReg_nonemergency.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\使用者\Desktop\高國鈞\NCU_python\Project\EdReg_0412\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\使用者\Desktop\高國鈞\Github\Project_EdReg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE25C80-77E6-40B5-A4FA-7434FFBD2C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F1073C-5248-4E02-858C-CDE02B0F37A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F276DA4-A4D2-4873-A959-DE0EC113F17D}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{9F276DA4-A4D2-4873-A959-DE0EC113F17D}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -100,10 +100,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ROUND(RAND()*(59.75-59.5)+59.5, 2)</t>
+    <t>position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>position</t>
+    <t>ROUND(RAND()*(59.75-59.51)+59.51, 2)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,11 +476,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59188F1-2934-4F42-96BE-6A5BF27C59D5}">
-  <dimension ref="A1:F314"/>
+  <dimension ref="A1:E314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G163" sqref="G163"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -493,7 +494,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -525,7 +526,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B60" ca="1" si="0" xml:space="preserve"> ROUND(RAND()*(60.02-59.98)+59.98, 2)</f>
-        <v>59.99</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -534,7 +535,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60.02</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,7 +544,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,7 +553,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -561,7 +562,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>59.98</v>
+        <v>60.02</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -570,7 +571,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -588,7 +589,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -597,7 +598,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>60.02</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,7 +607,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -615,7 +616,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,7 +625,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -633,7 +634,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>60.02</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,7 +643,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,7 +652,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>60.01</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +661,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -669,7 +670,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -678,7 +679,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>60.01</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,7 +697,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +715,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>60.01</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -723,7 +724,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +733,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -759,7 +760,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,7 +769,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,7 +778,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>60.01</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -786,7 +787,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,7 +796,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -813,7 +814,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>59.98</v>
+        <v>60.02</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +823,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>60.02</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -831,7 +832,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -840,7 +841,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -849,7 +850,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>60.02</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -858,7 +859,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>60.01</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +868,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,7 +886,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>60.01</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,7 +895,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>60.02</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -903,7 +904,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>59.98</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -912,7 +913,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>60.02</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -921,7 +922,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>60.02</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +931,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>60.01</v>
+        <v>60.02</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -939,7 +940,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -948,7 +949,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>59.99</v>
+        <v>60.02</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,7 +958,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>60.02</v>
+        <v>59.99</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -966,7 +967,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>59.98</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -975,7 +976,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>60.02</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,7 +1003,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="0"/>
-        <v>60.01</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,7 +1012,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1020,7 +1021,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,7 +1030,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,7 +1039,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="0"/>
-        <v>59.98</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1047,7 +1048,7 @@
       </c>
       <c r="B61">
         <f ca="1" xml:space="preserve"> ROUND(RAND()*(59.98-59.85)+59.85, 2)</f>
-        <v>59.89</v>
+        <v>59.93</v>
       </c>
       <c r="D61" t="s">
         <v>4</v>
@@ -1062,7 +1063,7 @@
       </c>
       <c r="B62">
         <f t="shared" ref="B62:B120" ca="1" si="1" xml:space="preserve"> ROUND(RAND()*(59.98-59.85)+59.85, 2)</f>
-        <v>59.97</v>
+        <v>59.95</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,7 +1072,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>59.9</v>
+        <v>59.89</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,7 +1081,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>59.85</v>
+        <v>59.89</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1090,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>59.88</v>
+        <v>59.85</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1098,7 +1099,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="1"/>
-        <v>59.92</v>
+        <v>59.9</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1107,7 +1108,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="1"/>
-        <v>59.92</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1117,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="1"/>
-        <v>59.87</v>
+        <v>59.95</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1125,7 +1126,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="1"/>
-        <v>59.9</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1134,7 +1135,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="1"/>
-        <v>59.85</v>
+        <v>59.87</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,7 +1144,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="1"/>
-        <v>59.87</v>
+        <v>59.92</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1152,7 +1153,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="1"/>
-        <v>59.86</v>
+        <v>59.96</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1161,7 +1162,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="1"/>
-        <v>59.92</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1170,7 +1171,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="1"/>
-        <v>59.95</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1179,7 +1180,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="1"/>
-        <v>59.88</v>
+        <v>59.86</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1189,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="1"/>
-        <v>59.96</v>
+        <v>59.91</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1197,7 +1198,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="1"/>
-        <v>59.91</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,7 +1207,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="1"/>
-        <v>59.89</v>
+        <v>59.96</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1215,7 +1216,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="1"/>
-        <v>59.89</v>
+        <v>59.91</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1224,7 +1225,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="1"/>
-        <v>59.96</v>
+        <v>59.94</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1233,7 +1234,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="1"/>
-        <v>59.93</v>
+        <v>59.94</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1242,7 +1243,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="1"/>
-        <v>59.92</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1251,7 +1252,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="1"/>
-        <v>59.89</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1260,7 +1261,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="1"/>
-        <v>59.9</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1269,7 +1270,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="1"/>
-        <v>59.92</v>
+        <v>59.89</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1278,7 +1279,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="1"/>
-        <v>59.91</v>
+        <v>59.89</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1287,7 +1288,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="1"/>
-        <v>59.86</v>
+        <v>59.92</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1296,7 +1297,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="1"/>
-        <v>59.97</v>
+        <v>59.92</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1305,7 +1306,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="1"/>
-        <v>59.98</v>
+        <v>59.97</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1314,7 +1315,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="1"/>
-        <v>59.92</v>
+        <v>59.88</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1323,7 +1324,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="1"/>
-        <v>59.86</v>
+        <v>59.94</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1332,7 +1333,7 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="1"/>
-        <v>59.94</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1341,7 +1342,7 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="1"/>
-        <v>59.9</v>
+        <v>59.88</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1350,7 +1351,7 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="1"/>
-        <v>59.91</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1359,7 +1360,7 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="1"/>
-        <v>59.9</v>
+        <v>59.86</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,7 +1369,7 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="1"/>
-        <v>59.97</v>
+        <v>59.93</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1377,7 +1378,7 @@
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="1"/>
-        <v>59.93</v>
+        <v>59.96</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1386,7 +1387,7 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="1"/>
-        <v>59.93</v>
+        <v>59.95</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1395,7 +1396,7 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="1"/>
-        <v>59.94</v>
+        <v>59.97</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,7 +1405,7 @@
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="1"/>
-        <v>59.92</v>
+        <v>59.96</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1413,7 +1414,7 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="1"/>
-        <v>59.89</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1431,7 +1432,7 @@
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="1"/>
-        <v>59.96</v>
+        <v>59.86</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1441,7 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="1"/>
-        <v>59.88</v>
+        <v>59.97</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1449,7 +1450,7 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="1"/>
-        <v>59.96</v>
+        <v>59.95</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1458,7 +1459,7 @@
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="1"/>
-        <v>59.87</v>
+        <v>59.97</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -1476,7 +1477,7 @@
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="1"/>
-        <v>59.9</v>
+        <v>59.95</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1494,7 +1495,7 @@
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="1"/>
-        <v>59.93</v>
+        <v>59.97</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -1503,7 +1504,7 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="1"/>
-        <v>59.88</v>
+        <v>59.9</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -1512,7 +1513,7 @@
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="1"/>
-        <v>59.85</v>
+        <v>59.91</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,7 +1522,7 @@
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="1"/>
-        <v>59.85</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,7 +1531,7 @@
       </c>
       <c r="B114">
         <f t="shared" ca="1" si="1"/>
-        <v>59.9</v>
+        <v>59.95</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,7 +1540,7 @@
       </c>
       <c r="B115">
         <f t="shared" ca="1" si="1"/>
-        <v>59.94</v>
+        <v>59.9</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,7 +1549,7 @@
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="1"/>
-        <v>59.88</v>
+        <v>59.97</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -1557,7 +1558,7 @@
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="1"/>
-        <v>59.92</v>
+        <v>59.86</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -1566,7 +1567,7 @@
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="1"/>
-        <v>59.85</v>
+        <v>59.94</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -1575,7 +1576,7 @@
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="1"/>
-        <v>59.89</v>
+        <v>59.85</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -1584,7 +1585,7 @@
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="1"/>
-        <v>59.93</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -1593,7 +1594,7 @@
       </c>
       <c r="B121">
         <f ca="1" xml:space="preserve"> ROUND(RAND()*(59.85-59.75)+59.75, 2)</f>
-        <v>59.82</v>
+        <v>59.83</v>
       </c>
       <c r="D121" t="s">
         <v>6</v>
@@ -1608,7 +1609,7 @@
       </c>
       <c r="B122">
         <f t="shared" ref="B122:B194" ca="1" si="2" xml:space="preserve"> ROUND(RAND()*(59.85-59.75)+59.75, 2)</f>
-        <v>59.79</v>
+        <v>59.78</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -1617,7 +1618,7 @@
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="2"/>
-        <v>59.79</v>
+        <v>59.75</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -1626,7 +1627,7 @@
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="2"/>
-        <v>59.79</v>
+        <v>59.77</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -1635,7 +1636,7 @@
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="2"/>
-        <v>59.8</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -1644,7 +1645,7 @@
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="2"/>
-        <v>59.83</v>
+        <v>59.84</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -1653,7 +1654,7 @@
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="2"/>
-        <v>59.76</v>
+        <v>59.81</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -1662,7 +1663,7 @@
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="2"/>
-        <v>59.76</v>
+        <v>59.85</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -1671,7 +1672,7 @@
       </c>
       <c r="B129">
         <f t="shared" ca="1" si="2"/>
-        <v>59.78</v>
+        <v>59.77</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -1680,7 +1681,7 @@
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="2"/>
-        <v>59.78</v>
+        <v>59.85</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -1689,7 +1690,7 @@
       </c>
       <c r="B131">
         <f t="shared" ca="1" si="2"/>
-        <v>59.81</v>
+        <v>59.8</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -1698,7 +1699,7 @@
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="2"/>
-        <v>59.82</v>
+        <v>59.83</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -1707,7 +1708,7 @@
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="2"/>
-        <v>59.85</v>
+        <v>59.81</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -1716,7 +1717,7 @@
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="2"/>
-        <v>59.77</v>
+        <v>59.83</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -1725,7 +1726,7 @@
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="2"/>
-        <v>59.76</v>
+        <v>59.78</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -1734,7 +1735,7 @@
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="2"/>
-        <v>59.77</v>
+        <v>59.81</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -1743,7 +1744,7 @@
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="2"/>
-        <v>59.85</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -1752,7 +1753,7 @@
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="2"/>
-        <v>59.76</v>
+        <v>59.78</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -1761,7 +1762,7 @@
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="2"/>
-        <v>59.8</v>
+        <v>59.83</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -1770,7 +1771,7 @@
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="2"/>
-        <v>59.83</v>
+        <v>59.78</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -1779,7 +1780,7 @@
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="2"/>
-        <v>59.8</v>
+        <v>59.83</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -1788,7 +1789,7 @@
       </c>
       <c r="B142">
         <f t="shared" ca="1" si="2"/>
-        <v>59.76</v>
+        <v>59.79</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -1797,7 +1798,7 @@
       </c>
       <c r="B143">
         <f t="shared" ca="1" si="2"/>
-        <v>59.75</v>
+        <v>59.83</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -1806,322 +1807,301 @@
       </c>
       <c r="B144">
         <f t="shared" ca="1" si="2"/>
+        <v>59.76</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>7</v>
+      </c>
+      <c r="B145">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.78</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>7</v>
+      </c>
+      <c r="B146">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>7</v>
+      </c>
+      <c r="B147">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.82</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>7</v>
+      </c>
+      <c r="B148">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>7</v>
+      </c>
+      <c r="B149">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.82</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>7</v>
+      </c>
+      <c r="B150">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.81</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>7</v>
+      </c>
+      <c r="B151">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.78</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>7</v>
+      </c>
+      <c r="B152">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.77</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>7</v>
+      </c>
+      <c r="B153">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.82</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>7</v>
+      </c>
+      <c r="B154">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.76</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>7</v>
+      </c>
+      <c r="B155">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.78</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>7</v>
+      </c>
+      <c r="B156">
+        <f t="shared" ca="1" si="2"/>
         <v>59.84</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>7</v>
-      </c>
-      <c r="B145">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.76</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>7</v>
-      </c>
-      <c r="B146">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.85</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>7</v>
-      </c>
-      <c r="B147">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.77</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>7</v>
-      </c>
-      <c r="B148">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157">
+        <f t="shared" ca="1" si="2"/>
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>7</v>
+      </c>
+      <c r="B158">
         <f t="shared" ca="1" si="2"/>
         <v>59.78</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>7</v>
-      </c>
-      <c r="B149">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.84</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>7</v>
-      </c>
-      <c r="B150">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.85</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>7</v>
-      </c>
-      <c r="B151">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.83</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>7</v>
-      </c>
-      <c r="B152">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.78</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>7</v>
-      </c>
-      <c r="B153">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.84</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>7</v>
-      </c>
-      <c r="B154">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.8</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>7</v>
-      </c>
-      <c r="B155">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.82</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>7</v>
-      </c>
-      <c r="B156">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.83</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>7</v>
-      </c>
-      <c r="B157">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.77</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>7</v>
-      </c>
-      <c r="B158">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.85</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B159" s="1">
-        <f t="shared" ref="B159:B165" ca="1" si="3" xml:space="preserve"> ROUND(RAND()*(59.75-59.5)+59.5, 2)</f>
-        <v>59.75</v>
+        <f ca="1" xml:space="preserve"> ROUND(RAND()*(59.75-59.51)+59.51, 2)</f>
+        <v>59.65</v>
       </c>
       <c r="D159" t="s">
-        <v>16</v>
-      </c>
-      <c r="F159">
-        <v>59.45</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B160" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="B160:B172" ca="1" si="3" xml:space="preserve"> ROUND(RAND()*(59.75-59.51)+59.51, 2)</f>
         <v>59.55</v>
       </c>
-      <c r="F160">
-        <v>59.45</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B161" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>59.69</v>
-      </c>
-      <c r="F161">
-        <v>59.45</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59.61</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B162" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>59.5</v>
-      </c>
-      <c r="F162">
-        <v>59.45</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59.52</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B163" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>59.53</v>
-      </c>
-      <c r="F163">
-        <v>59.5</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59.66</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B164" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>59.58</v>
-      </c>
-      <c r="F164">
-        <v>59.5</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59.67</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B165" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>59.6</v>
-      </c>
-      <c r="F165">
-        <v>59.5</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59.71</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B166" s="1">
-        <f ca="1" xml:space="preserve"> ROUND(RAND()*(59.75-59.5)+59.5, 2)</f>
-        <v>59.58</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>59.6</v>
       </c>
       <c r="E166" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B167" s="1">
-        <f t="shared" ref="B167:B172" ca="1" si="4" xml:space="preserve"> ROUND(RAND()*(59.75-59.5)+59.5, 2)</f>
-        <v>59.6</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="3"/>
+        <v>59.66</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B168" s="1">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>59.67</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B169" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>59.58</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="3"/>
+        <v>59.71</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B170" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>59.74</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="3"/>
+        <v>59.64</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B171" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>59.6</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="3"/>
+        <v>59.65</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B172" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>59.6</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="3"/>
+        <v>59.62</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>7</v>
       </c>
       <c r="B173">
         <f t="shared" ca="1" si="2"/>
-        <v>59.84</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>7</v>
       </c>
       <c r="B174">
         <f t="shared" ca="1" si="2"/>
+        <v>59.75</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B175">
+        <f t="shared" ca="1" si="2"/>
         <v>59.79</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>7</v>
-      </c>
-      <c r="B175">
-        <f t="shared" ca="1" si="2"/>
-        <v>59.75</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>7</v>
       </c>
       <c r="B176">
         <f t="shared" ca="1" si="2"/>
-        <v>59.84</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -2130,7 +2110,7 @@
       </c>
       <c r="B177">
         <f t="shared" ca="1" si="2"/>
-        <v>59.85</v>
+        <v>59.75</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -2139,7 +2119,7 @@
       </c>
       <c r="B178">
         <f t="shared" ca="1" si="2"/>
-        <v>59.75</v>
+        <v>59.79</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -2148,7 +2128,7 @@
       </c>
       <c r="B179">
         <f t="shared" ca="1" si="2"/>
-        <v>59.79</v>
+        <v>59.77</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -2157,7 +2137,7 @@
       </c>
       <c r="B180">
         <f t="shared" ca="1" si="2"/>
-        <v>59.76</v>
+        <v>59.83</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -2166,7 +2146,7 @@
       </c>
       <c r="B181">
         <f t="shared" ca="1" si="2"/>
-        <v>59.79</v>
+        <v>59.83</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -2175,7 +2155,7 @@
       </c>
       <c r="B182">
         <f t="shared" ca="1" si="2"/>
-        <v>59.8</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -2193,7 +2173,7 @@
       </c>
       <c r="B184">
         <f t="shared" ca="1" si="2"/>
-        <v>59.85</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -2202,7 +2182,7 @@
       </c>
       <c r="B185">
         <f t="shared" ca="1" si="2"/>
-        <v>59.78</v>
+        <v>59.8</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -2211,7 +2191,7 @@
       </c>
       <c r="B186">
         <f t="shared" ca="1" si="2"/>
-        <v>59.84</v>
+        <v>59.75</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -2220,7 +2200,7 @@
       </c>
       <c r="B187">
         <f t="shared" ca="1" si="2"/>
-        <v>59.79</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -2229,7 +2209,7 @@
       </c>
       <c r="B188">
         <f t="shared" ca="1" si="2"/>
-        <v>59.83</v>
+        <v>59.78</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -2238,7 +2218,7 @@
       </c>
       <c r="B189">
         <f t="shared" ca="1" si="2"/>
-        <v>59.79</v>
+        <v>59.81</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -2247,7 +2227,7 @@
       </c>
       <c r="B190">
         <f t="shared" ca="1" si="2"/>
-        <v>59.81</v>
+        <v>59.75</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -2265,7 +2245,7 @@
       </c>
       <c r="B192">
         <f t="shared" ca="1" si="2"/>
-        <v>59.8</v>
+        <v>59.76</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -2274,7 +2254,7 @@
       </c>
       <c r="B193">
         <f t="shared" ca="1" si="2"/>
-        <v>59.77</v>
+        <v>59.78</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -2283,7 +2263,7 @@
       </c>
       <c r="B194">
         <f t="shared" ca="1" si="2"/>
-        <v>59.8</v>
+        <v>59.81</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -2300,8 +2280,8 @@
         <v>1</v>
       </c>
       <c r="B196">
-        <f t="shared" ref="B196:B254" ca="1" si="5">ROUND(RAND()*(60.02-59.98)+59.98, 2)</f>
-        <v>59.99</v>
+        <f t="shared" ref="B196:B254" ca="1" si="4">ROUND(RAND()*(60.02-59.98)+59.98, 2)</f>
+        <v>60.02</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -2309,8 +2289,8 @@
         <v>1</v>
       </c>
       <c r="B197">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -2318,8 +2298,8 @@
         <v>1</v>
       </c>
       <c r="B198">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.98</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.01</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -2327,8 +2307,8 @@
         <v>1</v>
       </c>
       <c r="B199">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -2336,8 +2316,8 @@
         <v>1</v>
       </c>
       <c r="B200">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -2345,8 +2325,8 @@
         <v>1</v>
       </c>
       <c r="B201">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -2354,8 +2334,8 @@
         <v>1</v>
       </c>
       <c r="B202">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -2363,8 +2343,8 @@
         <v>1</v>
       </c>
       <c r="B203">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -2372,8 +2352,8 @@
         <v>1</v>
       </c>
       <c r="B204">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.98</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -2381,8 +2361,8 @@
         <v>1</v>
       </c>
       <c r="B205">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -2390,8 +2370,8 @@
         <v>1</v>
       </c>
       <c r="B206">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -2399,8 +2379,8 @@
         <v>1</v>
       </c>
       <c r="B207">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -2408,8 +2388,8 @@
         <v>1</v>
       </c>
       <c r="B208">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -2417,8 +2397,8 @@
         <v>1</v>
       </c>
       <c r="B209">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -2426,8 +2406,8 @@
         <v>1</v>
       </c>
       <c r="B210">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.01</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -2435,8 +2415,8 @@
         <v>1</v>
       </c>
       <c r="B211">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -2444,7 +2424,7 @@
         <v>1</v>
       </c>
       <c r="B212">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>60.01</v>
       </c>
     </row>
@@ -2453,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="B213">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>59.99</v>
       </c>
     </row>
@@ -2462,8 +2442,8 @@
         <v>1</v>
       </c>
       <c r="B214">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,8 +2451,8 @@
         <v>1</v>
       </c>
       <c r="B215">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -2480,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="B216">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>60.01</v>
       </c>
     </row>
@@ -2489,8 +2469,8 @@
         <v>1</v>
       </c>
       <c r="B217">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -2498,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="B218">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>60.01</v>
       </c>
     </row>
@@ -2507,8 +2487,8 @@
         <v>1</v>
       </c>
       <c r="B219">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -2516,8 +2496,8 @@
         <v>1</v>
       </c>
       <c r="B220">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -2525,8 +2505,8 @@
         <v>1</v>
       </c>
       <c r="B221">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.01</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -2534,8 +2514,8 @@
         <v>1</v>
       </c>
       <c r="B222">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -2543,8 +2523,8 @@
         <v>1</v>
       </c>
       <c r="B223">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -2552,8 +2532,8 @@
         <v>1</v>
       </c>
       <c r="B224">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.01</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -2561,8 +2541,8 @@
         <v>1</v>
       </c>
       <c r="B225">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.02</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -2570,7 +2550,7 @@
         <v>1</v>
       </c>
       <c r="B226">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>60</v>
       </c>
     </row>
@@ -2579,8 +2559,8 @@
         <v>1</v>
       </c>
       <c r="B227">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.02</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -2588,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="B228">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>59.99</v>
       </c>
     </row>
@@ -2597,8 +2577,8 @@
         <v>1</v>
       </c>
       <c r="B229">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -2606,8 +2586,8 @@
         <v>1</v>
       </c>
       <c r="B230">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.01</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -2615,8 +2595,8 @@
         <v>1</v>
       </c>
       <c r="B231">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.01</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -2624,8 +2604,8 @@
         <v>1</v>
       </c>
       <c r="B232">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -2633,8 +2613,8 @@
         <v>1</v>
       </c>
       <c r="B233">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -2642,8 +2622,8 @@
         <v>1</v>
       </c>
       <c r="B234">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -2651,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="B235">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>60</v>
       </c>
     </row>
@@ -2660,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="B236">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>60.02</v>
       </c>
     </row>
@@ -2669,8 +2649,8 @@
         <v>1</v>
       </c>
       <c r="B237">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -2678,8 +2658,8 @@
         <v>1</v>
       </c>
       <c r="B238">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,8 +2667,8 @@
         <v>1</v>
       </c>
       <c r="B239">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -2696,8 +2676,8 @@
         <v>1</v>
       </c>
       <c r="B240">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -2705,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="B241">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>59.99</v>
       </c>
     </row>
@@ -2714,7 +2694,7 @@
         <v>1</v>
       </c>
       <c r="B242">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>59.99</v>
       </c>
     </row>
@@ -2723,7 +2703,7 @@
         <v>1</v>
       </c>
       <c r="B243">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>60.02</v>
       </c>
     </row>
@@ -2732,8 +2712,8 @@
         <v>1</v>
       </c>
       <c r="B244">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.98</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -2741,8 +2721,8 @@
         <v>1</v>
       </c>
       <c r="B245">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.01</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -2750,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="B246">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>59.98</v>
       </c>
     </row>
@@ -2759,8 +2739,8 @@
         <v>1</v>
       </c>
       <c r="B247">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.01</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -2768,8 +2748,8 @@
         <v>1</v>
       </c>
       <c r="B248">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -2777,8 +2757,8 @@
         <v>1</v>
       </c>
       <c r="B249">
-        <f t="shared" ca="1" si="5"/>
-        <v>60.02</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -2786,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="B250">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>59.99</v>
       </c>
     </row>
@@ -2795,8 +2775,8 @@
         <v>1</v>
       </c>
       <c r="B251">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>60.01</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -2804,8 +2784,8 @@
         <v>1</v>
       </c>
       <c r="B252">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -2813,8 +2793,8 @@
         <v>1</v>
       </c>
       <c r="B253">
-        <f t="shared" ca="1" si="5"/>
-        <v>59.99</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.98</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -2822,8 +2802,8 @@
         <v>1</v>
       </c>
       <c r="B254">
-        <f t="shared" ca="1" si="5"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>59.99</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -2832,7 +2812,7 @@
       </c>
       <c r="B255">
         <f ca="1" xml:space="preserve"> ROUND(RAND()*(60.25-60.02)+60.02, 2)</f>
-        <v>60.23</v>
+        <v>60.11</v>
       </c>
       <c r="D255" t="s">
         <v>10</v>
@@ -2843,8 +2823,8 @@
         <v>13</v>
       </c>
       <c r="B256">
-        <f t="shared" ref="B256:B314" ca="1" si="6" xml:space="preserve"> ROUND(RAND()*(60.25-60.02)+60.02, 2)</f>
-        <v>60.1</v>
+        <f t="shared" ref="B256:B314" ca="1" si="5" xml:space="preserve"> ROUND(RAND()*(60.25-60.02)+60.02, 2)</f>
+        <v>60.22</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -2852,8 +2832,8 @@
         <v>13</v>
       </c>
       <c r="B257">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.2</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -2861,8 +2841,8 @@
         <v>13</v>
       </c>
       <c r="B258">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.06</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.19</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -2870,8 +2850,8 @@
         <v>13</v>
       </c>
       <c r="B259">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.24</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.2</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -2879,8 +2859,8 @@
         <v>13</v>
       </c>
       <c r="B260">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.12</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.17</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -2888,8 +2868,8 @@
         <v>13</v>
       </c>
       <c r="B261">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.24</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.16</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -2897,8 +2877,8 @@
         <v>13</v>
       </c>
       <c r="B262">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.23</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.18</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
@@ -2906,8 +2886,8 @@
         <v>13</v>
       </c>
       <c r="B263">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.14</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -2915,8 +2895,8 @@
         <v>13</v>
       </c>
       <c r="B264">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.11</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.09</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -2924,8 +2904,8 @@
         <v>13</v>
       </c>
       <c r="B265">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.16</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
@@ -2933,8 +2913,8 @@
         <v>13</v>
       </c>
       <c r="B266">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.04</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.12</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
@@ -2942,8 +2922,8 @@
         <v>13</v>
       </c>
       <c r="B267">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.03</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.2</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -2951,7 +2931,7 @@
         <v>13</v>
       </c>
       <c r="B268">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>60.05</v>
       </c>
     </row>
@@ -2960,8 +2940,8 @@
         <v>13</v>
       </c>
       <c r="B269">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.13</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.19</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
@@ -2969,8 +2949,8 @@
         <v>13</v>
       </c>
       <c r="B270">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.23</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -2978,8 +2958,8 @@
         <v>13</v>
       </c>
       <c r="B271">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.16</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
@@ -2987,8 +2967,8 @@
         <v>13</v>
       </c>
       <c r="B272">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.17</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
@@ -2996,8 +2976,8 @@
         <v>13</v>
       </c>
       <c r="B273">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.05</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.03</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -3005,8 +2985,8 @@
         <v>13</v>
       </c>
       <c r="B274">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.24</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
@@ -3014,8 +2994,8 @@
         <v>13</v>
       </c>
       <c r="B275">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.12</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.03</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
@@ -3023,8 +3003,8 @@
         <v>13</v>
       </c>
       <c r="B276">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.05</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.08</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -3032,8 +3012,8 @@
         <v>13</v>
       </c>
       <c r="B277">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.25</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.06</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -3041,8 +3021,8 @@
         <v>13</v>
       </c>
       <c r="B278">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.17</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
@@ -3050,8 +3030,8 @@
         <v>13</v>
       </c>
       <c r="B279">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.22</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -3059,8 +3039,8 @@
         <v>13</v>
       </c>
       <c r="B280">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.09</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.03</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
@@ -3068,8 +3048,8 @@
         <v>13</v>
       </c>
       <c r="B281">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.25</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.18</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
@@ -3077,8 +3057,8 @@
         <v>13</v>
       </c>
       <c r="B282">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.24</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -3086,8 +3066,8 @@
         <v>13</v>
       </c>
       <c r="B283">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.12</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.17</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
@@ -3095,8 +3075,8 @@
         <v>13</v>
       </c>
       <c r="B284">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.25</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,8 +3084,8 @@
         <v>13</v>
       </c>
       <c r="B285">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.08</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.05</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -3113,8 +3093,8 @@
         <v>13</v>
       </c>
       <c r="B286">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.08</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
@@ -3122,8 +3102,8 @@
         <v>13</v>
       </c>
       <c r="B287">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.05</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.16</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
@@ -3131,8 +3111,8 @@
         <v>13</v>
       </c>
       <c r="B288">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.14</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
@@ -3140,8 +3120,8 @@
         <v>13</v>
       </c>
       <c r="B289">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.08</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.19</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
@@ -3149,8 +3129,8 @@
         <v>13</v>
       </c>
       <c r="B290">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.14</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.07</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
@@ -3158,8 +3138,8 @@
         <v>13</v>
       </c>
       <c r="B291">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.14</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.16</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -3167,8 +3147,8 @@
         <v>13</v>
       </c>
       <c r="B292">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.17</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
@@ -3176,8 +3156,8 @@
         <v>13</v>
       </c>
       <c r="B293">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.05</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.08</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
@@ -3185,8 +3165,8 @@
         <v>13</v>
       </c>
       <c r="B294">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.18</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.21</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -3194,8 +3174,8 @@
         <v>13</v>
       </c>
       <c r="B295">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.16</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
@@ -3203,8 +3183,8 @@
         <v>13</v>
       </c>
       <c r="B296">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.14</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
@@ -3212,8 +3192,8 @@
         <v>13</v>
       </c>
       <c r="B297">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.13</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.19</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -3221,8 +3201,8 @@
         <v>13</v>
       </c>
       <c r="B298">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.23</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -3230,8 +3210,8 @@
         <v>13</v>
       </c>
       <c r="B299">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.06</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.14</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -3239,8 +3219,8 @@
         <v>13</v>
       </c>
       <c r="B300">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.25</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.13</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -3248,8 +3228,8 @@
         <v>13</v>
       </c>
       <c r="B301">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.11</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.17</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
@@ -3257,8 +3237,8 @@
         <v>13</v>
       </c>
       <c r="B302">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.12</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.06</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
@@ -3266,8 +3246,8 @@
         <v>13</v>
       </c>
       <c r="B303">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.14</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.16</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -3275,8 +3255,8 @@
         <v>13</v>
       </c>
       <c r="B304">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.23</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.15</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -3284,8 +3264,8 @@
         <v>13</v>
       </c>
       <c r="B305">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.02</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
@@ -3293,8 +3273,8 @@
         <v>13</v>
       </c>
       <c r="B306">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.06</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.11</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -3302,8 +3282,8 @@
         <v>13</v>
       </c>
       <c r="B307">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.19</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -3311,8 +3291,8 @@
         <v>13</v>
       </c>
       <c r="B308">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.24</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.12</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
@@ -3320,8 +3300,8 @@
         <v>13</v>
       </c>
       <c r="B309">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.23</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.1</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -3329,8 +3309,8 @@
         <v>13</v>
       </c>
       <c r="B310">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.06</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.19</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
@@ -3338,8 +3318,8 @@
         <v>13</v>
       </c>
       <c r="B311">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.03</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.14</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
@@ -3347,8 +3327,8 @@
         <v>13</v>
       </c>
       <c r="B312">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.17</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.05</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -3356,8 +3336,8 @@
         <v>13</v>
       </c>
       <c r="B313">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.08</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.19</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
@@ -3365,8 +3345,8 @@
         <v>13</v>
       </c>
       <c r="B314">
-        <f t="shared" ca="1" si="6"/>
-        <v>60.15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>60.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>